<commit_message>
Them cam bien van tay
</commit_message>
<xml_diff>
--- a/Tap lenh cho may.xlsx
+++ b/Tap lenh cho may.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4 ARDUINO\0 CODE\0 PROJECT\2111 TSTD\Tu_Sach_Tu_Dong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0AF408-D4C1-4E94-8A31-CFFF4DDD0663}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3B3DDE-E06D-4B7D-88B0-087CBBABF2F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tập lệnh" sheetId="1" r:id="rId1"/>
+    <sheet name="Ten Sach" sheetId="2" r:id="rId2"/>
+    <sheet name="Tên người" sheetId="4" r:id="rId3"/>
+    <sheet name="QR Code" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Stt</t>
   </si>
@@ -123,13 +124,28 @@
   </si>
   <si>
     <t>Đọc QR code từ cảm biến</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên </t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>Đọc vân tay</t>
+  </si>
+  <si>
+    <t>VTDK</t>
+  </si>
+  <si>
+    <t>Đăng ký vân tay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +181,13 @@
       <color theme="1"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -208,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -218,9 +241,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -233,6 +253,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -274,9 +298,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1218749</xdr:colOff>
+      <xdr:colOff>1035959</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1021920</xdr:rowOff>
+      <xdr:rowOff>841920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -299,7 +323,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2339340" y="784860"/>
-          <a:ext cx="913949" cy="900000"/>
+          <a:ext cx="731159" cy="720000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -317,9 +341,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1181939</xdr:colOff>
+      <xdr:colOff>1001939</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1021919</xdr:rowOff>
+      <xdr:rowOff>841919</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -343,7 +367,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="891539" y="784859"/>
-          <a:ext cx="900000" cy="900000"/>
+          <a:ext cx="720000" cy="720000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -361,9 +385,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1140630</xdr:colOff>
+      <xdr:colOff>967368</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1044780</xdr:rowOff>
+      <xdr:rowOff>864780</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -387,7 +411,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3733800" y="807720"/>
-          <a:ext cx="866310" cy="900000"/>
+          <a:ext cx="693048" cy="720000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -399,15 +423,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>289559</xdr:colOff>
+      <xdr:colOff>289560</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>129539</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1175043</xdr:colOff>
+      <xdr:colOff>997947</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1029539</xdr:rowOff>
+      <xdr:rowOff>849539</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -430,8 +454,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5173979" y="792479"/>
-          <a:ext cx="885484" cy="900000"/>
+          <a:off x="5173980" y="792479"/>
+          <a:ext cx="708387" cy="720000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -449,9 +473,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1174319</xdr:colOff>
+      <xdr:colOff>994319</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>991439</xdr:rowOff>
+      <xdr:rowOff>811439</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -475,7 +499,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="883919" y="2377439"/>
-          <a:ext cx="900000" cy="900000"/>
+          <a:ext cx="720000" cy="720000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -493,9 +517,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1181939</xdr:colOff>
+      <xdr:colOff>1001939</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>999059</xdr:rowOff>
+      <xdr:rowOff>819059</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -519,7 +543,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2316479" y="2385059"/>
-          <a:ext cx="900000" cy="900000"/>
+          <a:ext cx="720000" cy="720000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -537,9 +561,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1199560</xdr:colOff>
+      <xdr:colOff>1017560</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>1014300</xdr:rowOff>
+      <xdr:rowOff>834300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -563,7 +587,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3749040" y="2400300"/>
-          <a:ext cx="910000" cy="900000"/>
+          <a:ext cx="728000" cy="720000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -581,9 +605,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1174319</xdr:colOff>
+      <xdr:colOff>994319</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>1006679</xdr:rowOff>
+      <xdr:rowOff>826679</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -607,7 +631,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5158739" y="2392679"/>
-          <a:ext cx="900000" cy="900000"/>
+          <a:ext cx="720000" cy="720000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -885,7 +909,7 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,13 +922,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="21" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="4" spans="2:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -1048,19 +1072,27 @@
       <c r="B14" s="1">
         <v>10</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>11</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
@@ -1128,11 +1160,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59F516C-1112-4388-8BAF-9141B9E34029}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD20D5B-05E1-48AA-A7EA-8C28763C15D9}">
   <dimension ref="B1:I7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1147,72 +1197,72 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="2:9" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="2:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="2:9" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>